<commit_message>
test case2 5 dof ddqn v2
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/train_results/DDQN_outputs/case2/6/DDQN-6-variable-20230521-064836/models/tested_state_traj/tested_state_traj_1_0-A-10.xlsx
+++ b/dynamics/src/dynamics/train_results/DDQN_outputs/case2/6/DDQN-6-variable-20230521-064836/models/tested_state_traj/tested_state_traj_1_0-A-10.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,31 +423,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" t="n">
-        <v>70.49444578511469</v>
+        <v>72.33599344369235</v>
       </c>
       <c r="C1" t="n">
         <v>1</v>
       </c>
       <c r="D1" t="n">
-        <v>0.02169049215491954</v>
+        <v>0.02134025532994542</v>
       </c>
       <c r="E1" t="n">
-        <v>28.13539322953832</v>
+        <v>26.19194824819854</v>
       </c>
       <c r="F1" t="n">
-        <v>21.86460677046168</v>
+        <v>23.80805175180146</v>
       </c>
       <c r="G1" t="n">
         <v>30.4</v>
       </c>
       <c r="I1" t="n">
-        <v>5.1</v>
+        <v>25.3</v>
       </c>
       <c r="J1" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="2">
@@ -455,19 +455,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>70.49444578511469</v>
+        <v>72.33599344369235</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.02169049215491954</v>
+        <v>0.02134025532994542</v>
       </c>
       <c r="E2" t="n">
-        <v>28.13539322953832</v>
+        <v>26.19194824819854</v>
       </c>
       <c r="F2" t="n">
-        <v>21.86460677046168</v>
+        <v>23.80805175180146</v>
       </c>
       <c r="G2" t="n">
         <v>50.6</v>
@@ -476,7 +476,7 @@
         <v>25.3</v>
       </c>
       <c r="J2" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="3">
@@ -484,19 +484,19 @@
         <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>70.68790170528636</v>
+        <v>73.14513819719954</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.02111428542157593</v>
+        <v>0.02085744766964147</v>
       </c>
       <c r="E3" t="n">
-        <v>28.13539322953832</v>
+        <v>26.19194824819854</v>
       </c>
       <c r="F3" t="n">
-        <v>20.86460677046168</v>
+        <v>22.80805175180146</v>
       </c>
       <c r="G3" t="n">
         <v>50.6</v>
@@ -505,7 +505,7 @@
         <v>25.3</v>
       </c>
       <c r="J3" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="4">
@@ -513,19 +513,19 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>69.53226729077859</v>
+        <v>72.6462875200349</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0.02051707444013215</v>
+        <v>0.02035102115440001</v>
       </c>
       <c r="E4" t="n">
-        <v>28.13539322953832</v>
+        <v>26.19194824819854</v>
       </c>
       <c r="F4" t="n">
-        <v>19.86460677046168</v>
+        <v>21.80805175180146</v>
       </c>
       <c r="G4" t="n">
         <v>50.6</v>
@@ -534,7 +534,7 @@
         <v>25.3</v>
       </c>
       <c r="J4" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="5">
@@ -542,19 +542,19 @@
         <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>69.59791605257698</v>
+        <v>73.41709546472336</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>0.01989833943509195</v>
+        <v>0.02082945626278331</v>
       </c>
       <c r="E5" t="n">
-        <v>28.13539322953832</v>
+        <v>26.19194824819854</v>
       </c>
       <c r="F5" t="n">
-        <v>18.86460677046168</v>
+        <v>20.80805175180146</v>
       </c>
       <c r="G5" t="n">
         <v>50.6</v>
@@ -563,7 +563,7 @@
         <v>25.3</v>
       </c>
       <c r="J5" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="6">
@@ -571,19 +571,19 @@
         <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>69.6112503030252</v>
+        <v>73.05836701639915</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>0.01925836303326388</v>
+        <v>0.02025853058378118</v>
       </c>
       <c r="E6" t="n">
-        <v>28.13539322953832</v>
+        <v>26.19194824819854</v>
       </c>
       <c r="F6" t="n">
-        <v>17.86460677046168</v>
+        <v>19.80805175180146</v>
       </c>
       <c r="G6" t="n">
         <v>50.6</v>
@@ -592,7 +592,7 @@
         <v>25.3</v>
       </c>
       <c r="J6" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="7">
@@ -600,19 +600,19 @@
         <v>0</v>
       </c>
       <c r="B7" t="n">
-        <v>69.56683863692008</v>
+        <v>72.64702396216171</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.0196680202921729</v>
       </c>
       <c r="E7" t="n">
-        <v>28.13539322953832</v>
+        <v>26.19194824819854</v>
       </c>
       <c r="F7" t="n">
-        <v>16.86460677046168</v>
+        <v>18.80805175180146</v>
       </c>
       <c r="G7" t="n">
         <v>50.6</v>
@@ -621,7 +621,7 @@
         <v>25.3</v>
       </c>
       <c r="J7" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="8">
@@ -629,28 +629,28 @@
         <v>0</v>
       </c>
       <c r="B8" t="n">
-        <v>69.56683863692008</v>
+        <v>72.18306990523536</v>
       </c>
       <c r="C8" t="n">
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01905857850574538</v>
       </c>
       <c r="E8" t="n">
-        <v>28.13539322953832</v>
+        <v>26.19194824819854</v>
       </c>
       <c r="F8" t="n">
-        <v>16.86460677046168</v>
+        <v>17.80805175180146</v>
       </c>
       <c r="G8" t="n">
-        <v>70</v>
+        <v>50.6</v>
       </c>
       <c r="I8" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J8" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="9">
@@ -658,28 +658,28 @@
         <v>0</v>
       </c>
       <c r="B9" t="n">
-        <v>69.56683863692008</v>
+        <v>70.41284128799957</v>
       </c>
       <c r="C9" t="n">
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01936787546980214</v>
       </c>
       <c r="E9" t="n">
-        <v>28.13539322953832</v>
+        <v>26.19194824819854</v>
       </c>
       <c r="F9" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G9" t="n">
-        <v>70</v>
+        <v>50.6</v>
       </c>
       <c r="I9" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J9" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="10">
@@ -687,28 +687,28 @@
         <v>0</v>
       </c>
       <c r="B10" t="n">
-        <v>69.56683863692008</v>
+        <v>70.41284128799957</v>
       </c>
       <c r="C10" t="n">
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01936787546980214</v>
       </c>
       <c r="E10" t="n">
-        <v>28.13539322953832</v>
+        <v>26.19194824819854</v>
       </c>
       <c r="F10" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G10" t="n">
         <v>70</v>
       </c>
       <c r="I10" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J10" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="11">
@@ -716,28 +716,28 @@
         <v>0</v>
       </c>
       <c r="B11" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C11" t="n">
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E11" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F11" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G11" t="n">
         <v>70</v>
       </c>
       <c r="I11" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J11" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="12">
@@ -745,28 +745,28 @@
         <v>0</v>
       </c>
       <c r="B12" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C12" t="n">
         <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E12" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F12" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G12" t="n">
         <v>70</v>
       </c>
       <c r="I12" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J12" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="13">
@@ -774,28 +774,28 @@
         <v>0</v>
       </c>
       <c r="B13" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C13" t="n">
         <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E13" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F13" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G13" t="n">
         <v>70</v>
       </c>
       <c r="I13" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J13" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="14">
@@ -803,28 +803,28 @@
         <v>0</v>
       </c>
       <c r="B14" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C14" t="n">
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E14" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F14" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G14" t="n">
         <v>70</v>
       </c>
       <c r="I14" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J14" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="15">
@@ -832,28 +832,28 @@
         <v>0</v>
       </c>
       <c r="B15" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C15" t="n">
         <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E15" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F15" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G15" t="n">
         <v>70</v>
       </c>
       <c r="I15" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J15" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="16">
@@ -861,28 +861,28 @@
         <v>0</v>
       </c>
       <c r="B16" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C16" t="n">
         <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E16" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F16" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G16" t="n">
         <v>70</v>
       </c>
       <c r="I16" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J16" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="17">
@@ -890,28 +890,28 @@
         <v>0</v>
       </c>
       <c r="B17" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C17" t="n">
         <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E17" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F17" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G17" t="n">
         <v>70</v>
       </c>
       <c r="I17" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J17" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="18">
@@ -919,28 +919,28 @@
         <v>0</v>
       </c>
       <c r="B18" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C18" t="n">
         <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E18" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F18" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G18" t="n">
         <v>70</v>
       </c>
       <c r="I18" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J18" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="19">
@@ -948,28 +948,28 @@
         <v>0</v>
       </c>
       <c r="B19" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C19" t="n">
         <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E19" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F19" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G19" t="n">
         <v>70</v>
       </c>
       <c r="I19" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J19" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="20">
@@ -977,28 +977,28 @@
         <v>0</v>
       </c>
       <c r="B20" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C20" t="n">
         <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E20" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F20" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G20" t="n">
         <v>70</v>
       </c>
       <c r="I20" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J20" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="21">
@@ -1006,28 +1006,28 @@
         <v>0</v>
       </c>
       <c r="B21" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C21" t="n">
         <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E21" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F21" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G21" t="n">
         <v>70</v>
       </c>
       <c r="I21" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J21" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="22">
@@ -1035,28 +1035,28 @@
         <v>0</v>
       </c>
       <c r="B22" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C22" t="n">
         <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E22" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F22" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G22" t="n">
         <v>70</v>
       </c>
       <c r="I22" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J22" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="23">
@@ -1064,28 +1064,28 @@
         <v>0</v>
       </c>
       <c r="B23" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C23" t="n">
         <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E23" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F23" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G23" t="n">
         <v>70</v>
       </c>
       <c r="I23" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J23" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="24">
@@ -1093,28 +1093,28 @@
         <v>0</v>
       </c>
       <c r="B24" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C24" t="n">
         <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E24" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F24" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G24" t="n">
         <v>70</v>
       </c>
       <c r="I24" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J24" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="25">
@@ -1122,28 +1122,28 @@
         <v>0</v>
       </c>
       <c r="B25" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C25" t="n">
         <v>1</v>
       </c>
       <c r="D25" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E25" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F25" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G25" t="n">
         <v>70</v>
       </c>
       <c r="I25" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J25" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="26">
@@ -1151,28 +1151,28 @@
         <v>0</v>
       </c>
       <c r="B26" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C26" t="n">
         <v>1</v>
       </c>
       <c r="D26" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E26" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F26" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G26" t="n">
         <v>70</v>
       </c>
       <c r="I26" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J26" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="27">
@@ -1180,28 +1180,28 @@
         <v>0</v>
       </c>
       <c r="B27" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C27" t="n">
         <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E27" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F27" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G27" t="n">
         <v>70</v>
       </c>
       <c r="I27" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J27" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="28">
@@ -1209,28 +1209,28 @@
         <v>0</v>
       </c>
       <c r="B28" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C28" t="n">
         <v>1</v>
       </c>
       <c r="D28" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E28" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F28" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G28" t="n">
         <v>70</v>
       </c>
       <c r="I28" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J28" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="29">
@@ -1238,28 +1238,28 @@
         <v>0</v>
       </c>
       <c r="B29" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C29" t="n">
         <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E29" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F29" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G29" t="n">
         <v>70</v>
       </c>
       <c r="I29" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J29" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="30">
@@ -1267,28 +1267,28 @@
         <v>0</v>
       </c>
       <c r="B30" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C30" t="n">
         <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E30" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F30" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G30" t="n">
         <v>70</v>
       </c>
       <c r="I30" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J30" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="31">
@@ -1296,28 +1296,28 @@
         <v>0</v>
       </c>
       <c r="B31" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C31" t="n">
         <v>1</v>
       </c>
       <c r="D31" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E31" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F31" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G31" t="n">
         <v>70</v>
       </c>
       <c r="I31" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J31" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="32">
@@ -1325,28 +1325,28 @@
         <v>0</v>
       </c>
       <c r="B32" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C32" t="n">
         <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E32" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F32" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G32" t="n">
         <v>70</v>
       </c>
       <c r="I32" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J32" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="33">
@@ -1354,28 +1354,28 @@
         <v>0</v>
       </c>
       <c r="B33" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C33" t="n">
         <v>1</v>
       </c>
       <c r="D33" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E33" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F33" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G33" t="n">
         <v>70</v>
       </c>
       <c r="I33" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J33" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="34">
@@ -1383,28 +1383,28 @@
         <v>0</v>
       </c>
       <c r="B34" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C34" t="n">
         <v>1</v>
       </c>
       <c r="D34" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E34" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F34" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G34" t="n">
         <v>70</v>
       </c>
       <c r="I34" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J34" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="35">
@@ -1412,28 +1412,28 @@
         <v>0</v>
       </c>
       <c r="B35" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C35" t="n">
         <v>1</v>
       </c>
       <c r="D35" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E35" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F35" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G35" t="n">
         <v>70</v>
       </c>
       <c r="I35" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J35" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="36">
@@ -1441,28 +1441,28 @@
         <v>0</v>
       </c>
       <c r="B36" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C36" t="n">
         <v>1</v>
       </c>
       <c r="D36" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E36" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F36" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G36" t="n">
         <v>70</v>
       </c>
       <c r="I36" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J36" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="37">
@@ -1470,28 +1470,28 @@
         <v>0</v>
       </c>
       <c r="B37" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C37" t="n">
         <v>1</v>
       </c>
       <c r="D37" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E37" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F37" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G37" t="n">
         <v>70</v>
       </c>
       <c r="I37" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J37" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="38">
@@ -1499,28 +1499,28 @@
         <v>0</v>
       </c>
       <c r="B38" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C38" t="n">
         <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E38" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F38" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G38" t="n">
         <v>70</v>
       </c>
       <c r="I38" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J38" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="39">
@@ -1528,28 +1528,28 @@
         <v>0</v>
       </c>
       <c r="B39" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C39" t="n">
         <v>1</v>
       </c>
       <c r="D39" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E39" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F39" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G39" t="n">
         <v>70</v>
       </c>
       <c r="I39" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J39" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="40">
@@ -1557,28 +1557,28 @@
         <v>0</v>
       </c>
       <c r="B40" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C40" t="n">
         <v>1</v>
       </c>
       <c r="D40" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E40" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F40" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G40" t="n">
         <v>70</v>
       </c>
       <c r="I40" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J40" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="41">
@@ -1586,28 +1586,28 @@
         <v>0</v>
       </c>
       <c r="B41" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C41" t="n">
         <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E41" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F41" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G41" t="n">
         <v>70</v>
       </c>
       <c r="I41" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J41" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="42">
@@ -1615,28 +1615,28 @@
         <v>0</v>
       </c>
       <c r="B42" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C42" t="n">
         <v>1</v>
       </c>
       <c r="D42" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E42" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F42" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G42" t="n">
         <v>70</v>
       </c>
       <c r="I42" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J42" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="43">
@@ -1644,28 +1644,28 @@
         <v>0</v>
       </c>
       <c r="B43" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C43" t="n">
         <v>1</v>
       </c>
       <c r="D43" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E43" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F43" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G43" t="n">
         <v>70</v>
       </c>
       <c r="I43" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J43" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="44">
@@ -1673,28 +1673,28 @@
         <v>0</v>
       </c>
       <c r="B44" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C44" t="n">
         <v>1</v>
       </c>
       <c r="D44" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E44" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F44" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G44" t="n">
         <v>70</v>
       </c>
       <c r="I44" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J44" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="45">
@@ -1702,28 +1702,28 @@
         <v>0</v>
       </c>
       <c r="B45" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C45" t="n">
         <v>1</v>
       </c>
       <c r="D45" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E45" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F45" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G45" t="n">
         <v>70</v>
       </c>
       <c r="I45" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J45" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="46">
@@ -1731,28 +1731,28 @@
         <v>0</v>
       </c>
       <c r="B46" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C46" t="n">
         <v>1</v>
       </c>
       <c r="D46" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E46" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F46" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G46" t="n">
         <v>70</v>
       </c>
       <c r="I46" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J46" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="47">
@@ -1760,28 +1760,28 @@
         <v>0</v>
       </c>
       <c r="B47" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C47" t="n">
         <v>1</v>
       </c>
       <c r="D47" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E47" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F47" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G47" t="n">
         <v>70</v>
       </c>
       <c r="I47" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J47" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="48">
@@ -1789,28 +1789,28 @@
         <v>0</v>
       </c>
       <c r="B48" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C48" t="n">
         <v>1</v>
       </c>
       <c r="D48" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E48" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F48" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G48" t="n">
         <v>70</v>
       </c>
       <c r="I48" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J48" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="49">
@@ -1818,28 +1818,28 @@
         <v>0</v>
       </c>
       <c r="B49" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C49" t="n">
         <v>1</v>
       </c>
       <c r="D49" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E49" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F49" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G49" t="n">
         <v>70</v>
       </c>
       <c r="I49" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J49" t="n">
-        <v>25.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="50">
@@ -1847,27 +1847,827 @@
         <v>0</v>
       </c>
       <c r="B50" t="n">
-        <v>69.56683863692008</v>
+        <v>73.22537652927181</v>
       </c>
       <c r="C50" t="n">
         <v>1</v>
       </c>
       <c r="D50" t="n">
-        <v>0.01859602732464842</v>
+        <v>0.01966940723649535</v>
       </c>
       <c r="E50" t="n">
-        <v>28.13539322953832</v>
+        <v>27.19194824819854</v>
       </c>
       <c r="F50" t="n">
-        <v>16.86460677046168</v>
+        <v>16.80805175180146</v>
       </c>
       <c r="G50" t="n">
         <v>70</v>
       </c>
       <c r="I50" t="n">
-        <v>44.7</v>
+        <v>25.3</v>
       </c>
       <c r="J50" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="I51" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J51" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="I52" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J52" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="I53" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J53" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="I54" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J54" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="I55" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J55" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="I56" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J56" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="I57" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J57" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="I58" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J58" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="I59" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J59" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="I60" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J60" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="I61" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J61" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="I62" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J62" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="I63" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J63" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="I64" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J64" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="I65" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J65" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="I66" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J66" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="I67" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J67" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="I68" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J68" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="I69" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J69" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="I70" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J70" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="I71" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J71" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="I72" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J72" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="I73" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J73" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="I74" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J74" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="I75" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J75" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="I76" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J76" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="I77" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J77" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="I78" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J78" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="I79" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J79" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="I80" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J80" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="I81" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J81" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="I82" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J82" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="I83" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J83" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="I84" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J84" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="I85" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J85" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="I86" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J86" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="I87" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J87" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="I88" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J88" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="I89" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J89" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="I90" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J90" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="I91" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J91" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="I92" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J92" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="I93" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J93" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="I94" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J94" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="I95" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J95" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="I96" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J96" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="I97" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J97" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="I98" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J98" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="I99" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J99" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="I100" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J100" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="I101" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="J101" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="I102" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J102" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="I103" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J103" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="I104" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J104" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="I105" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J105" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="I106" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J106" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="I107" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J107" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="I108" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J108" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="I109" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J109" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="I110" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J110" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="I111" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J111" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="I112" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J112" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="I113" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J113" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="I114" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J114" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="I115" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J115" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="I116" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J116" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="I117" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J117" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="I118" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J118" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="I119" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J119" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="I120" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J120" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="I121" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J121" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="I122" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J122" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="I123" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J123" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="I124" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J124" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="I125" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J125" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="I126" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J126" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="I127" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J127" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="I128" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J128" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="I129" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J129" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="I130" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J130" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="I131" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J131" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="I132" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J132" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="I133" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J133" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="I134" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J134" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="I135" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J135" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="I136" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J136" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="I137" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J137" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="I138" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J138" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="I139" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J139" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="I140" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J140" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="I141" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J141" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="I142" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J142" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="I143" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J143" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="I144" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J144" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="I145" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J145" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="I146" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J146" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="I147" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J147" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="I148" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J148" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="I149" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J149" t="n">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="I150" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="J150" t="n">
         <v>25.3</v>
       </c>
     </row>

</xml_diff>